<commit_message>
- Add plotly and mapbox
</commit_message>
<xml_diff>
--- a/core/static/fixtures/mindmap-v3.xlsx
+++ b/core/static/fixtures/mindmap-v3.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tetrapak-my.sharepoint.com/personal/zaturnerp_tetrapak_com/Documents/@Archive/2021/Writing/SA Inequality/sankey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Workspace/Software/Projects/saffaction/core/static/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="424" documentId="8_{2478B322-9C28-4625-ACCD-328E8AB548BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D71B2EA4-D5C3-42B1-826B-272107A02B01}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5B03B1-0266-AB41-9A49-7EB5800DB08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MindMap" sheetId="1" r:id="rId1"/>
     <sheet name="Stages" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
     <sheet name="Terminology" sheetId="4" r:id="rId4"/>
-    <sheet name="Next" sheetId="2" r:id="rId5"/>
-    <sheet name="solutions" sheetId="6" r:id="rId6"/>
+    <sheet name="sankey" sheetId="6" r:id="rId5"/>
+    <sheet name="agents" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="290">
   <si>
     <t>Financial data --- big challenge! long delays, lots of privacy issues (salaries), contractal/legal vendor challenges, NDAs (?), and stigma ("employees shouldn't know how much we spend on marketing because then they'll want better canteen")</t>
   </si>
@@ -733,30 +733,6 @@
     <t>Digital transformation</t>
   </si>
   <si>
-    <t>Value chain mapping</t>
-  </si>
-  <si>
-    <t>Matrix with difficuly of solutions</t>
-  </si>
-  <si>
-    <t>Visual representation? How do we visualise the problem space?</t>
-  </si>
-  <si>
-    <t>More ideas from other indistries where projects failed?</t>
-  </si>
-  <si>
-    <t>Going through the powerpoints templates slides we can repurpose</t>
-  </si>
-  <si>
-    <t>Which are big issues / frequently responsible for failure</t>
-  </si>
-  <si>
-    <t>Which are linked</t>
-  </si>
-  <si>
-    <t>What does the solutions to these look like?</t>
-  </si>
-  <si>
     <t>JDP</t>
   </si>
   <si>
@@ -842,15 +818,6 @@
   </si>
   <si>
     <t>Tax incentives for private schools in areas that are in need of better schools</t>
-  </si>
-  <si>
-    <t>People With Means (PWM)</t>
-  </si>
-  <si>
-    <t>Communities (schools, churches etc.)</t>
-  </si>
-  <si>
-    <t>Private Enterprise</t>
   </si>
   <si>
     <t>National Government</t>
@@ -941,14 +908,35 @@
     <t xml:space="preserve">Free online training of TB, HIV and treatment literacies </t>
   </si>
   <si>
-    <t>NGOs, Charities, and Other Organizations</t>
+    <t>People with Means (PWM)</t>
+  </si>
+  <si>
+    <t>Families</t>
+  </si>
+  <si>
+    <t>NGOs, Charities  &amp; Other Organizations</t>
+  </si>
+  <si>
+    <t>Communities (Schools, Churches etc.)</t>
+  </si>
+  <si>
+    <t>Large Enterprises</t>
+  </si>
+  <si>
+    <t>Private Equity</t>
+  </si>
+  <si>
+    <t>Small-Medium Sized Businesses</t>
+  </si>
+  <si>
+    <t>Trade Unions &amp; Associations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1015,13 +1003,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1041,7 +1022,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1128,6 +1109,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,7 +1294,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1404,6 +1391,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1437,15 +1433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -1769,9 +1757,9 @@
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="33" width="5.6328125" customWidth="1"/>
+    <col min="1" max="33" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:25">
@@ -1983,11 +1971,11 @@
       <c r="H20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L20" s="42" t="s">
+      <c r="L20" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="M20" s="43"/>
-      <c r="N20" s="44"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="47"/>
       <c r="S20" t="s">
         <v>48</v>
       </c>
@@ -1997,9 +1985,9 @@
       <c r="H21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L21" s="45"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="47"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="50"/>
       <c r="S21" t="s">
         <v>50</v>
       </c>
@@ -2009,9 +1997,9 @@
       <c r="H22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L22" s="48"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="53"/>
       <c r="S22" t="s">
         <v>52</v>
       </c>
@@ -2174,7 +2162,7 @@
       </c>
       <c r="O38" s="6"/>
     </row>
-    <row r="39" spans="7:20" ht="15.5">
+    <row r="39" spans="7:20" ht="16">
       <c r="H39" s="3"/>
       <c r="I39" s="4" t="s">
         <v>87</v>
@@ -2208,7 +2196,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="7:20" ht="15.5">
+    <row r="43" spans="7:20" ht="16">
       <c r="H43" s="2" t="s">
         <v>94</v>
       </c>
@@ -2424,20 +2412,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="9" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection activeCell="M24" sqref="M24"/>
+      <selection pane="topRight" activeCell="M24" sqref="M24"/>
+      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
+      <selection pane="bottomRight" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.453125" customWidth="1"/>
-    <col min="4" max="4" width="33.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="5" style="16" customWidth="1"/>
-    <col min="10" max="13" width="22.453125" style="16" customWidth="1"/>
-    <col min="15" max="22" width="3.81640625" customWidth="1"/>
-    <col min="23" max="23" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="22.5" style="16" customWidth="1"/>
+    <col min="15" max="22" width="3.83203125" customWidth="1"/>
+    <col min="23" max="23" width="2.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22">
@@ -2464,25 +2453,25 @@
         <v>146</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>147</v>
       </c>
       <c r="J3" s="20"/>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-    </row>
-    <row r="4" spans="2:22" ht="29">
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+    </row>
+    <row r="4" spans="2:22" ht="32">
       <c r="E4" s="35">
         <v>0.2</v>
       </c>
@@ -3430,10 +3419,10 @@
   <dimension ref="B7:C69"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
@@ -3628,13 +3617,13 @@
   <dimension ref="C2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="5.81640625" customWidth="1"/>
-    <col min="4" max="4" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="4" max="4" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:7">
@@ -3655,11 +3644,11 @@
       <c r="D6" t="s">
         <v>221</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
     </row>
     <row r="7" spans="3:7">
       <c r="C7" t="s">
@@ -3668,9 +3657,9 @@
       <c r="D7" t="s">
         <v>223</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
     </row>
     <row r="8" spans="3:7">
       <c r="C8" t="s">
@@ -3737,681 +3726,691 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E38435-76FB-5442-BF90-357BA83A0FCA}">
-  <dimension ref="C5:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4E4CBE-549C-3549-89EA-CC482C9B1D9A}">
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29.83203125" style="41" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="3:3">
+    <row r="1" spans="1:4" ht="16">
+      <c r="A1" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="64">
+      <c r="A2" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="64">
+      <c r="A3" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="64">
+      <c r="A4" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="64">
+      <c r="A5" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>242</v>
+      </c>
       <c r="C5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="64">
+      <c r="A6" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>242</v>
+      </c>
       <c r="C6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48">
+      <c r="A7" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="C7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48">
+      <c r="A8" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>243</v>
+      </c>
       <c r="C8" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="32">
+      <c r="A9" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="C9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="32">
+      <c r="A10" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>244</v>
+      </c>
       <c r="C10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="32">
+      <c r="A11" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="80">
+      <c r="A12" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>246</v>
+      </c>
       <c r="C12" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32">
+      <c r="A13" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" t="s">
+        <v>288</v>
+      </c>
+      <c r="D13" s="56"/>
+    </row>
+    <row r="14" spans="1:4" ht="32">
+      <c r="A14" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="32">
+      <c r="A15" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32">
+      <c r="A16" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="48">
+      <c r="A17" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>250</v>
+      </c>
       <c r="C17" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="48">
+      <c r="A18" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>250</v>
+      </c>
       <c r="C18" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="48">
+      <c r="A19" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>250</v>
+      </c>
       <c r="C19" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="32">
+      <c r="A20" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="C20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="32">
+      <c r="A21" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="C21" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="32">
+      <c r="A22" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="C22" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="48">
+      <c r="A23" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="C23" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="48">
+      <c r="A24" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="C24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="80">
+      <c r="A25" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="C25" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="32">
+      <c r="A26" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="C26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="32">
+      <c r="A27" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="C27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="32">
+      <c r="A28" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="64">
+      <c r="A29" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="64">
+      <c r="A30" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="C30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="48">
+      <c r="A31" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="C31" t="s">
+        <v>282</v>
+      </c>
+      <c r="D31" s="56"/>
+    </row>
+    <row r="32" spans="1:4" ht="32">
+      <c r="A32" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="C32" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="48">
+      <c r="A33" s="40" t="s">
         <v>239</v>
       </c>
+      <c r="B33" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="C33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="48">
+      <c r="A34" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="C34" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="80">
+      <c r="A35" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="C35" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="80">
+      <c r="A36" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="C36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="48">
+      <c r="A37" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="48">
+      <c r="A38" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="48">
+      <c r="A39" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="48">
+      <c r="A40" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="64">
+      <c r="A41" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="64">
+      <c r="A42" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="48">
+      <c r="A43" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="48">
+      <c r="A44" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="48">
+      <c r="A45" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="32">
+      <c r="A46" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="32">
+      <c r="A47" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="B47" s="40" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="64">
+      <c r="A48" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="B48" s="42" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="48">
+      <c r="A49" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="B49" s="42" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="64">
+      <c r="A50" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="32">
+      <c r="A51" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="B51" s="42" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16">
+      <c r="A52" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="B52" s="42" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="32">
+      <c r="A53" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="48">
+      <c r="A54" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="48">
+      <c r="A55" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B55" s="43" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="64">
+      <c r="A56" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B56" s="42" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="64">
+      <c r="A57" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B57" s="43" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="32">
+      <c r="A58" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B58" s="43" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="32">
+      <c r="A59" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B59" s="43" t="s">
+        <v>281</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB2B8036-7DD5-264F-8545-BA65DAB64877}">
+          <x14:formula1>
+            <xm:f>agents!$A$1:$A$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C135</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4E4CBE-549C-3549-89EA-CC482C9B1D9A}">
-  <dimension ref="A1:C55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2BCBAF-D6AA-AA44-A9B8-1D8AAF8B42C9}">
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.90625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="39" t="s">
-        <v>243</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="58">
-      <c r="A2" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="C2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="58">
-      <c r="A3" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="C3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="58">
-      <c r="A4" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>250</v>
-      </c>
-      <c r="C4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="58">
-      <c r="A5" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>250</v>
-      </c>
-      <c r="C5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.5">
-      <c r="A6" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="C6" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="29">
-      <c r="A7" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="C7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="29">
-      <c r="A8" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="C8" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="29">
-      <c r="A9" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>253</v>
-      </c>
-      <c r="C9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="87">
-      <c r="A10" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>254</v>
-      </c>
-      <c r="C10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="29">
-      <c r="A11" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>256</v>
-      </c>
-      <c r="C11" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="29">
-      <c r="A12" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>255</v>
-      </c>
-      <c r="C12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="29">
-      <c r="A13" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>257</v>
-      </c>
-      <c r="C13" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="29">
-      <c r="A14" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>257</v>
-      </c>
-      <c r="C14" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="43.5">
-      <c r="A15" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>258</v>
-      </c>
-      <c r="C15" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="29">
-      <c r="A16" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>259</v>
-      </c>
-      <c r="C16" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="43.5">
-      <c r="A17" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="C17" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="43.5">
-      <c r="A18" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="C18" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="43.5">
-      <c r="A19" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="C19" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="43.5">
-      <c r="A20" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="C20" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="87">
-      <c r="A21" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>254</v>
-      </c>
-      <c r="C21" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="29">
-      <c r="A22" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B22" s="40" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>261</v>
       </c>
-      <c r="C22" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="29">
-      <c r="A23" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>261</v>
-      </c>
-      <c r="C23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="29">
-      <c r="A24" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>261</v>
-      </c>
-      <c r="C24" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="58">
-      <c r="A25" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>262</v>
-      </c>
-      <c r="C25" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="58">
-      <c r="A26" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>262</v>
-      </c>
-      <c r="C26" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="43.5">
-      <c r="A27" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>263</v>
-      </c>
-      <c r="C27" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="29">
-      <c r="A28" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>264</v>
-      </c>
-      <c r="C28" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="43.5">
-      <c r="A29" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="C29" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="43.5">
-      <c r="A30" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="C30" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="72.5">
-      <c r="A31" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B31" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="C31" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="72.5">
-      <c r="A32" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B32" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="C32" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="43.5">
-      <c r="A33" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B33" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="C33" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="43.5">
-      <c r="A34" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B34" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="C34" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="43.5">
-      <c r="A35" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B35" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="C35" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="43.5">
-      <c r="A36" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B36" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="C36" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="58">
-      <c r="A37" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B37" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="C37" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="58">
-      <c r="A38" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B38" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="C38" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="43.5">
-      <c r="A39" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B39" s="40" t="s">
-        <v>263</v>
-      </c>
-      <c r="C39" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="43.5">
-      <c r="A40" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B40" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="C40" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="43.5">
-      <c r="A41" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B41" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="C41" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="29">
-      <c r="A42" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>279</v>
-      </c>
-      <c r="C42" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="29">
-      <c r="A43" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="B43" s="40" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="58">
-      <c r="A44" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="B44" s="53" t="s">
-        <v>280</v>
-      </c>
-      <c r="C44" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="43.5">
-      <c r="A45" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="B45" s="53" t="s">
-        <v>281</v>
-      </c>
-      <c r="C45" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="72.5">
-      <c r="A46" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="B46" s="53" t="s">
-        <v>282</v>
-      </c>
-      <c r="C46" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="29">
-      <c r="A47" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="B47" s="53" t="s">
-        <v>283</v>
-      </c>
-      <c r="C47" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="B48" s="53" t="s">
-        <v>284</v>
-      </c>
-      <c r="C48" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="29">
-      <c r="A49" s="41" t="s">
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>285</v>
       </c>
-      <c r="B49" s="54" t="s">
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>286</v>
       </c>
-      <c r="C49" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="42">
-      <c r="A50" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="B50" s="55" t="s">
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>287</v>
       </c>
-      <c r="C50" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="43.5">
-      <c r="A51" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="B51" s="54" t="s">
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>288</v>
       </c>
-      <c r="C51" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="58">
-      <c r="A52" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="B52" s="53" t="s">
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
         <v>289</v>
       </c>
-      <c r="C52" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="58">
-      <c r="A53" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="B53" s="54" t="s">
-        <v>290</v>
-      </c>
-      <c r="C53" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="43.5">
-      <c r="A54" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="B54" s="54" t="s">
-        <v>291</v>
-      </c>
-      <c r="C54" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="29">
-      <c r="A55" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="B55" s="54" t="s">
-        <v>292</v>
-      </c>
-      <c r="C55" t="s">
-        <v>269</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4574,18 +4573,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4607,18 +4606,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{003386C0-D252-4BC4-8CE6-DF32C4FA2773}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3935BDD-DC1E-4E58-B2A6-24C00395DAEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{003386C0-D252-4BC4-8CE6-DF32C4FA2773}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>